<commit_message>
updated biomass equation and notebook B bound calculations
</commit_message>
<xml_diff>
--- a/data/13c_mfa/INCA model 12212023_summary_GR.xlsx
+++ b/data/13c_mfa/INCA model 12212023_summary_GR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrettroell/yarrowia_eflux2/data/13c_mfa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2137D601-6849-E643-8EF4-631DB974FBAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876888DC-5345-3D47-A77B-119BE6A39D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15280" yWindow="500" windowWidth="35920" windowHeight="25640" xr2:uid="{AAE6672A-B131-4F2E-90C4-18E461171EDC}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="335">
   <si>
     <t>ID</t>
   </si>
@@ -1274,6 +1274,12 @@
   </si>
   <si>
     <t>Pathway</t>
+  </si>
+  <si>
+    <t>SUCD2_u6m or SUCD1m</t>
+  </si>
+  <si>
+    <t>AKGDam</t>
   </si>
 </sst>
 </file>
@@ -2374,7 +2380,7 @@
   <dimension ref="A1:O73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3617,7 +3623,7 @@
         <v>64</v>
       </c>
       <c r="D28" s="81" t="s">
-        <v>256</v>
+        <v>334</v>
       </c>
       <c r="E28" s="81" t="s">
         <v>300</v>
@@ -3662,7 +3668,7 @@
         <v>66</v>
       </c>
       <c r="D29" s="81" t="s">
-        <v>257</v>
+        <v>333</v>
       </c>
       <c r="E29" s="81" t="s">
         <v>301</v>

</xml_diff>